<commit_message>
Segundo commit, se comenzo el arbol 4 y faltaron las predicciones de ese arbol
</commit_message>
<xml_diff>
--- a/Diccionario de datos.xlsx
+++ b/Diccionario de datos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA98749-DD16-478D-9442-0C0EFC65493A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A96A1BD-9B08-4652-AFC4-0980E7AC516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1440,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC88276-E443-47E5-8C66-CC4AFCD30076}">
   <dimension ref="A2:C143"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A99" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -2357,7 +2357,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="A94" s="18" t="s">
         <v>125</v>
       </c>
       <c r="B94" s="13">
@@ -2513,7 +2513,7 @@
       <c r="B110" s="13">
         <v>2</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="18" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
       <c r="B113" s="13">
         <v>5</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="18" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2596,7 +2596,7 @@
       <c r="B119" s="13">
         <v>5</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2663,7 +2663,7 @@
       <c r="B126" s="13">
         <v>3</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" s="18" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2672,7 +2672,7 @@
       <c r="B127" s="13">
         <v>4</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="18" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2772,7 +2772,7 @@
       <c r="B137" s="13">
         <v>1</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C137" s="18" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
3er commit, se termino las predicciones con los arboles de decisión y su documentación
</commit_message>
<xml_diff>
--- a/Diccionario de datos.xlsx
+++ b/Diccionario de datos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A96A1BD-9B08-4652-AFC4-0980E7AC516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3300F56-D1E9-423D-8923-C98DC15B65D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1440,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC88276-E443-47E5-8C66-CC4AFCD30076}">
   <dimension ref="A2:C143"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -2113,7 +2113,7 @@
       <c r="B68" s="13">
         <v>2</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="18" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2131,7 +2131,7 @@
       <c r="B70" s="13">
         <v>4</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="18" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2504,7 +2504,7 @@
       <c r="B109" s="13">
         <v>1</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="18" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2522,7 +2522,7 @@
       <c r="B111" s="13">
         <v>3</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="18" t="s">
         <v>133</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ultimo commit, proyecto finalizado, se implemento las redes neuronales
</commit_message>
<xml_diff>
--- a/Diccionario de datos.xlsx
+++ b/Diccionario de datos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A235856-40EA-45EB-9423-D2824DFACD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D3E9F5-5813-45F8-B413-48A39B55C566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1440,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC88276-E443-47E5-8C66-CC4AFCD30076}">
   <dimension ref="A2:C143"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A96" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1934,7 @@
       <c r="B49" s="13">
         <v>1</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="18" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>